<commit_message>
AutoCommit_22 марта 2024 г. 10:07:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SibNout2023\Downloads\KipFin_Lab_2023-24_Git0\2ИСИП-522\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C9" sqref="C9"/>
+      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -555,8 +555,12 @@
         <v>1</v>
       </c>
       <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
+      <c r="D4" s="2">
+        <v>5</v>
+      </c>
+      <c r="E4" s="2">
+        <v>5</v>
+      </c>
       <c r="F4" s="2"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
@@ -857,8 +861,12 @@
       <c r="C22" s="2">
         <v>5</v>
       </c>
-      <c r="D22" s="2"/>
-      <c r="E22" s="2"/>
+      <c r="D22" s="2">
+        <v>5</v>
+      </c>
+      <c r="E22" s="2">
+        <v>5</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_29 марта 2024 г. 10:04:00_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F22" sqref="F22"/>
+      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -659,7 +659,9 @@
       <c r="E10" s="2">
         <v>5</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="2">
+        <v>5</v>
+      </c>
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
@@ -723,12 +725,18 @@
         <v>11</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
+      <c r="D14" s="2">
+        <v>5</v>
+      </c>
       <c r="E14" s="2">
         <v>5</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
+      <c r="F14" s="2">
+        <v>5</v>
+      </c>
+      <c r="G14" s="2">
+        <v>5</v>
+      </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
     </row>
@@ -763,8 +771,12 @@
       <c r="C16" s="2">
         <v>5</v>
       </c>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
+      <c r="D16" s="2">
+        <v>5</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
+      </c>
       <c r="F16" s="2"/>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
@@ -827,8 +839,12 @@
       <c r="C20" s="2">
         <v>5</v>
       </c>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
+      <c r="D20" s="2">
+        <v>5</v>
+      </c>
+      <c r="E20" s="2">
+        <v>5</v>
+      </c>
       <c r="F20" s="2"/>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_4 апреля 2024 г. 13:55:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F20" sqref="F20"/>
+      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -636,8 +636,12 @@
       <c r="C9" s="2">
         <v>5</v>
       </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
+      <c r="D9" s="2">
+        <v>5</v>
+      </c>
+      <c r="E9" s="2">
+        <v>5</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 9:24:02_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F9" sqref="F9"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -603,9 +603,15 @@
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="C7" s="2">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2">
+        <v>5</v>
+      </c>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -982,11 +988,21 @@
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2"/>
-      <c r="D28" s="2"/>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
+      <c r="C28" s="2">
+        <v>5</v>
+      </c>
+      <c r="D28" s="2">
+        <v>5</v>
+      </c>
+      <c r="E28" s="2">
+        <v>5</v>
+      </c>
+      <c r="F28" s="2">
+        <v>5</v>
+      </c>
+      <c r="G28" s="2">
+        <v>5</v>
+      </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
     </row>

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 9:27:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
+      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -926,10 +926,18 @@
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2"/>
-      <c r="D24" s="2"/>
-      <c r="E24" s="2"/>
-      <c r="F24" s="2"/>
+      <c r="C24" s="2">
+        <v>5</v>
+      </c>
+      <c r="D24" s="2">
+        <v>5</v>
+      </c>
+      <c r="E24" s="2">
+        <v>5</v>
+      </c>
+      <c r="F24" s="2">
+        <v>5</v>
+      </c>
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 9:35:24_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -504,7 +504,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G24" sqref="G24"/>
+      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -719,8 +719,12 @@
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
+      <c r="C13" s="2">
+        <v>5</v>
+      </c>
+      <c r="D13" s="2">
+        <v>5</v>
+      </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
@@ -799,9 +803,15 @@
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
+      <c r="C17" s="2">
+        <v>5</v>
+      </c>
+      <c r="D17" s="2">
+        <v>5</v>
+      </c>
+      <c r="E17" s="2">
+        <v>5</v>
+      </c>
       <c r="F17" s="2"/>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
@@ -832,8 +842,12 @@
       <c r="C19" s="2">
         <v>5</v>
       </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
+      <c r="D19" s="2">
+        <v>5</v>
+      </c>
+      <c r="E19" s="2">
+        <v>5</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_5 апреля 2024 г. 9:52:34_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F19" sqref="F19"/>
+      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -588,8 +588,12 @@
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
+      <c r="C6" s="2">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2">
+        <v>5</v>
+      </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
       <c r="G6" s="2"/>
@@ -692,7 +696,9 @@
       <c r="E11" s="2">
         <v>5</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="2">
+        <v>4</v>
+      </c>
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
@@ -928,8 +934,12 @@
       <c r="E23" s="2">
         <v>5</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="G23" s="2"/>
+      <c r="F23" s="2">
+        <v>5</v>
+      </c>
+      <c r="G23" s="2">
+        <v>5</v>
+      </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
     </row>
@@ -1065,10 +1075,18 @@
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
+      <c r="C31" s="2">
+        <v>4</v>
+      </c>
+      <c r="D31" s="2">
+        <v>4</v>
+      </c>
+      <c r="E31" s="2">
+        <v>4</v>
+      </c>
+      <c r="F31" s="2">
+        <v>4</v>
+      </c>
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_10 апреля 2024 г. 14:55:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G11" sqref="G11"/>
+      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -628,9 +628,15 @@
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
+      <c r="C8" s="2">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2">
+        <v>5</v>
+      </c>
+      <c r="E8" s="2">
+        <v>5</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
@@ -710,10 +716,18 @@
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
-      <c r="F12" s="2"/>
+      <c r="C12" s="2">
+        <v>5</v>
+      </c>
+      <c r="D12" s="2">
+        <v>5</v>
+      </c>
+      <c r="E12" s="2">
+        <v>5</v>
+      </c>
+      <c r="F12" s="2">
+        <v>5</v>
+      </c>
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
@@ -1005,10 +1019,18 @@
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2"/>
-      <c r="D27" s="2"/>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
+      <c r="C27" s="2">
+        <v>5</v>
+      </c>
+      <c r="D27" s="2">
+        <v>5</v>
+      </c>
+      <c r="E27" s="2">
+        <v>5</v>
+      </c>
+      <c r="F27" s="2">
+        <v>5</v>
+      </c>
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 11:01:18_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -501,10 +501,10 @@
   <dimension ref="A1:I33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F27" sqref="F27"/>
+      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -790,7 +790,9 @@
       <c r="E15" s="2">
         <v>5</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="2">
+        <v>5</v>
+      </c>
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
@@ -811,7 +813,9 @@
       <c r="E16" s="2">
         <v>5</v>
       </c>
-      <c r="F16" s="2"/>
+      <c r="F16" s="2">
+        <v>5</v>
+      </c>
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
@@ -868,7 +872,9 @@
       <c r="E19" s="2">
         <v>5</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="2">
+        <v>5</v>
+      </c>
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 13:05:58_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>2ИСИП-522: Теория вероятностей и математическая статистика (Сибирев И. В.) - II семестр</t>
   </si>
@@ -124,6 +124,12 @@
   </si>
   <si>
     <t>ДЗ_5</t>
+  </si>
+  <si>
+    <t>сумма</t>
+  </si>
+  <si>
+    <t>тк</t>
   </si>
 </sst>
 </file>
@@ -156,7 +162,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -179,11 +185,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -193,6 +210,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -498,13 +518,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I33"/>
+  <dimension ref="A1:K33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L14" sqref="L14"/>
+      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -514,12 +534,12 @@
     <col min="3" max="9" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -537,8 +557,14 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
-    </row>
-    <row r="3" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J2" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -547,7 +573,7 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -565,8 +591,15 @@
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-    </row>
-    <row r="5" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J4">
+        <f>SUM(C4:I4)</f>
+        <v>10</v>
+      </c>
+      <c r="K4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -580,8 +613,15 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
-    </row>
-    <row r="6" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J5">
+        <f t="shared" ref="J5:J32" si="0">SUM(C5:I5)</f>
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -599,8 +639,15 @@
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
-    </row>
-    <row r="7" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J6">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -620,8 +667,15 @@
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
-    </row>
-    <row r="8" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -641,8 +695,15 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-    </row>
-    <row r="9" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -662,8 +723,15 @@
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
-    </row>
-    <row r="10" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -685,8 +753,15 @@
       <c r="G10" s="2"/>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
-    </row>
-    <row r="11" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J10">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -708,8 +783,15 @@
       <c r="G11" s="2"/>
       <c r="H11" s="2"/>
       <c r="I11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J11">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="K11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -731,8 +813,15 @@
       <c r="G12" s="2"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
-    </row>
-    <row r="13" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J12">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -750,8 +839,15 @@
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
-    </row>
-    <row r="14" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J13">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -773,8 +869,15 @@
       </c>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
-    </row>
-    <row r="15" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -796,8 +899,15 @@
       <c r="G15" s="2"/>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
-    </row>
-    <row r="16" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -819,8 +929,15 @@
       <c r="G16" s="2"/>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
-    </row>
-    <row r="17" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -840,8 +957,15 @@
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
-    </row>
-    <row r="18" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -855,8 +979,15 @@
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
-    </row>
-    <row r="19" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -878,8 +1009,15 @@
       <c r="G19" s="2"/>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
-    </row>
-    <row r="20" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -899,8 +1037,15 @@
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
-    </row>
-    <row r="21" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -916,8 +1061,15 @@
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
-    </row>
-    <row r="22" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J21">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K21">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -937,8 +1089,15 @@
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
-    </row>
-    <row r="23" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -962,8 +1121,15 @@
       </c>
       <c r="H23" s="2"/>
       <c r="I23" s="2"/>
-    </row>
-    <row r="24" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J23">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -985,8 +1151,15 @@
       <c r="G24" s="2"/>
       <c r="H24" s="2"/>
       <c r="I24" s="2"/>
-    </row>
-    <row r="25" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J24">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -1002,8 +1175,15 @@
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
-    </row>
-    <row r="26" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J25">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="K25">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
@@ -1017,8 +1197,15 @@
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
-    </row>
-    <row r="27" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J26">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
@@ -1040,8 +1227,15 @@
       <c r="G27" s="2"/>
       <c r="H27" s="2"/>
       <c r="I27" s="2"/>
-    </row>
-    <row r="28" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="K27">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
@@ -1065,8 +1259,15 @@
       </c>
       <c r="H28" s="2"/>
       <c r="I28" s="2"/>
-    </row>
-    <row r="29" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="K28">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
@@ -1080,8 +1281,15 @@
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
-    </row>
-    <row r="30" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K29">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
@@ -1095,8 +1303,15 @@
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="K30">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
@@ -1118,8 +1333,15 @@
       <c r="G31" s="2"/>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
-    </row>
-    <row r="32" spans="1:9" ht="13" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="K31">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
@@ -1139,6 +1361,13 @@
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
+      <c r="J32">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="K32">
+        <v>4</v>
+      </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C33" s="3"/>
@@ -1151,6 +1380,18 @@
     </row>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
+  <conditionalFormatting sqref="J4:J32">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 20:16:20_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -154,12 +154,18 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -200,7 +206,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -212,6 +218,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -518,13 +527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K33"/>
+  <dimension ref="A1:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="K31" sqref="K31"/>
+      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -534,12 +543,12 @@
     <col min="3" max="9" width="5.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="13" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="13" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="29" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" ht="29" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>30</v>
       </c>
@@ -564,7 +573,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -573,21 +582,25 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2">
-        <v>5</v>
-      </c>
-      <c r="F4" s="2"/>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5">
+        <v>5</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0</v>
+      </c>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -598,18 +611,29 @@
       <c r="K4">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="C5" s="5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
       <c r="I5" s="2"/>
@@ -620,22 +644,29 @@
       <c r="K5">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="C6" s="5">
+        <v>5</v>
+      </c>
+      <c r="D6" s="5">
+        <v>5</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
       <c r="I6" s="2"/>
@@ -646,24 +677,29 @@
       <c r="K6">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="2">
-        <v>5</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
-      </c>
-      <c r="E7" s="2">
-        <v>5</v>
-      </c>
-      <c r="F7" s="2"/>
+      <c r="C7" s="5">
+        <v>5</v>
+      </c>
+      <c r="D7" s="5">
+        <v>5</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
+      </c>
+      <c r="F7" s="5">
+        <v>0</v>
+      </c>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="I7" s="2"/>
@@ -674,24 +710,29 @@
       <c r="K7">
         <v>4</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="2">
-        <v>5</v>
-      </c>
-      <c r="D8" s="2">
-        <v>5</v>
-      </c>
-      <c r="E8" s="2">
-        <v>5</v>
-      </c>
-      <c r="F8" s="2"/>
+      <c r="C8" s="5">
+        <v>5</v>
+      </c>
+      <c r="D8" s="5">
+        <v>5</v>
+      </c>
+      <c r="E8" s="5">
+        <v>5</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0</v>
+      </c>
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
@@ -702,24 +743,29 @@
       <c r="K8">
         <v>4</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="2">
-        <v>5</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
-      </c>
-      <c r="E9" s="2">
-        <v>5</v>
-      </c>
-      <c r="F9" s="2"/>
+      <c r="C9" s="5">
+        <v>5</v>
+      </c>
+      <c r="D9" s="5">
+        <v>5</v>
+      </c>
+      <c r="E9" s="5">
+        <v>5</v>
+      </c>
+      <c r="F9" s="5">
+        <v>0</v>
+      </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
@@ -730,24 +776,27 @@
       <c r="K9">
         <v>4</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="2">
-        <v>5</v>
-      </c>
-      <c r="D10" s="2">
-        <v>5</v>
-      </c>
-      <c r="E10" s="2">
-        <v>5</v>
-      </c>
-      <c r="F10" s="2">
+      <c r="C10" s="5">
+        <v>5</v>
+      </c>
+      <c r="D10" s="5">
+        <v>5</v>
+      </c>
+      <c r="E10" s="5">
+        <v>5</v>
+      </c>
+      <c r="F10" s="5">
         <v>5</v>
       </c>
       <c r="G10" s="2"/>
@@ -760,24 +809,27 @@
       <c r="K10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>8</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
-      </c>
-      <c r="E11" s="2">
-        <v>5</v>
-      </c>
-      <c r="F11" s="2">
+      <c r="C11" s="5">
+        <v>5</v>
+      </c>
+      <c r="D11" s="5">
+        <v>5</v>
+      </c>
+      <c r="E11" s="5">
+        <v>5</v>
+      </c>
+      <c r="F11" s="5">
         <v>4</v>
       </c>
       <c r="G11" s="2"/>
@@ -790,24 +842,27 @@
       <c r="K11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>9</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C12" s="2">
-        <v>5</v>
-      </c>
-      <c r="D12" s="2">
-        <v>5</v>
-      </c>
-      <c r="E12" s="2">
-        <v>5</v>
-      </c>
-      <c r="F12" s="2">
+      <c r="C12" s="5">
+        <v>5</v>
+      </c>
+      <c r="D12" s="5">
+        <v>5</v>
+      </c>
+      <c r="E12" s="5">
+        <v>5</v>
+      </c>
+      <c r="F12" s="5">
         <v>5</v>
       </c>
       <c r="G12" s="2"/>
@@ -820,22 +875,29 @@
       <c r="K12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>10</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="2">
-        <v>5</v>
-      </c>
-      <c r="D13" s="2">
-        <v>5</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
+      <c r="C13" s="5">
+        <v>5</v>
+      </c>
+      <c r="D13" s="5">
+        <v>5</v>
+      </c>
+      <c r="E13" s="5">
+        <v>0</v>
+      </c>
+      <c r="F13" s="5">
+        <v>0</v>
+      </c>
       <c r="G13" s="2"/>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
@@ -846,22 +908,27 @@
       <c r="K13">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2">
-        <v>5</v>
-      </c>
-      <c r="E14" s="2">
-        <v>5</v>
-      </c>
-      <c r="F14" s="2">
+      <c r="C14" s="5">
+        <v>0</v>
+      </c>
+      <c r="D14" s="5">
+        <v>5</v>
+      </c>
+      <c r="E14" s="5">
+        <v>5</v>
+      </c>
+      <c r="F14" s="5">
         <v>5</v>
       </c>
       <c r="G14" s="2">
@@ -876,24 +943,27 @@
       <c r="K14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>12</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2">
-        <v>5</v>
-      </c>
-      <c r="D15" s="2">
-        <v>5</v>
-      </c>
-      <c r="E15" s="2">
-        <v>5</v>
-      </c>
-      <c r="F15" s="2">
+      <c r="C15" s="5">
+        <v>5</v>
+      </c>
+      <c r="D15" s="5">
+        <v>5</v>
+      </c>
+      <c r="E15" s="5">
+        <v>5</v>
+      </c>
+      <c r="F15" s="5">
         <v>5</v>
       </c>
       <c r="G15" s="2"/>
@@ -906,24 +976,27 @@
       <c r="K15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>13</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="2">
-        <v>5</v>
-      </c>
-      <c r="D16" s="2">
-        <v>5</v>
-      </c>
-      <c r="E16" s="2">
-        <v>5</v>
-      </c>
-      <c r="F16" s="2">
+      <c r="C16" s="5">
+        <v>5</v>
+      </c>
+      <c r="D16" s="5">
+        <v>5</v>
+      </c>
+      <c r="E16" s="5">
+        <v>5</v>
+      </c>
+      <c r="F16" s="5">
         <v>5</v>
       </c>
       <c r="G16" s="2"/>
@@ -936,24 +1009,29 @@
       <c r="K16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2">
-        <v>5</v>
-      </c>
-      <c r="D17" s="2">
-        <v>5</v>
-      </c>
-      <c r="E17" s="2">
-        <v>5</v>
-      </c>
-      <c r="F17" s="2"/>
+      <c r="C17" s="5">
+        <v>5</v>
+      </c>
+      <c r="D17" s="5">
+        <v>5</v>
+      </c>
+      <c r="E17" s="5">
+        <v>5</v>
+      </c>
+      <c r="F17" s="5">
+        <v>0</v>
+      </c>
       <c r="G17" s="2"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
@@ -964,18 +1042,29 @@
       <c r="K17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="C18" s="5">
+        <v>0</v>
+      </c>
+      <c r="D18" s="5">
+        <v>0</v>
+      </c>
+      <c r="E18" s="5">
+        <v>0</v>
+      </c>
+      <c r="F18" s="5">
+        <v>0</v>
+      </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
       <c r="I18" s="2"/>
@@ -986,24 +1075,27 @@
       <c r="K18">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="2">
-        <v>5</v>
-      </c>
-      <c r="D19" s="2">
-        <v>5</v>
-      </c>
-      <c r="E19" s="2">
-        <v>5</v>
-      </c>
-      <c r="F19" s="2">
+      <c r="C19" s="5">
+        <v>5</v>
+      </c>
+      <c r="D19" s="5">
+        <v>5</v>
+      </c>
+      <c r="E19" s="5">
+        <v>5</v>
+      </c>
+      <c r="F19" s="5">
         <v>5</v>
       </c>
       <c r="G19" s="2"/>
@@ -1016,24 +1108,29 @@
       <c r="K19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="2">
-        <v>5</v>
-      </c>
-      <c r="D20" s="2">
-        <v>5</v>
-      </c>
-      <c r="E20" s="2">
-        <v>5</v>
-      </c>
-      <c r="F20" s="2"/>
+      <c r="C20" s="5">
+        <v>5</v>
+      </c>
+      <c r="D20" s="5">
+        <v>5</v>
+      </c>
+      <c r="E20" s="5">
+        <v>5</v>
+      </c>
+      <c r="F20" s="5">
+        <v>0</v>
+      </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
@@ -1044,20 +1141,29 @@
       <c r="K20">
         <v>4</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="2">
-        <v>5</v>
-      </c>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="C21" s="5">
+        <v>5</v>
+      </c>
+      <c r="D21" s="5">
+        <v>0</v>
+      </c>
+      <c r="E21" s="5">
+        <v>0</v>
+      </c>
+      <c r="F21" s="5">
+        <v>0</v>
+      </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
@@ -1068,24 +1174,29 @@
       <c r="K21">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>19</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="2">
-        <v>5</v>
-      </c>
-      <c r="D22" s="2">
-        <v>5</v>
-      </c>
-      <c r="E22" s="2">
-        <v>5</v>
-      </c>
-      <c r="F22" s="2"/>
+      <c r="C22" s="5">
+        <v>5</v>
+      </c>
+      <c r="D22" s="5">
+        <v>5</v>
+      </c>
+      <c r="E22" s="5">
+        <v>5</v>
+      </c>
+      <c r="F22" s="5">
+        <v>0</v>
+      </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
@@ -1096,24 +1207,27 @@
       <c r="K22">
         <v>4</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="2">
-        <v>5</v>
-      </c>
-      <c r="D23" s="2">
-        <v>5</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="F23" s="2">
+      <c r="C23" s="5">
+        <v>5</v>
+      </c>
+      <c r="D23" s="5">
+        <v>5</v>
+      </c>
+      <c r="E23" s="5">
+        <v>5</v>
+      </c>
+      <c r="F23" s="5">
         <v>5</v>
       </c>
       <c r="G23" s="2">
@@ -1128,24 +1242,27 @@
       <c r="K23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>21</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="2">
-        <v>5</v>
-      </c>
-      <c r="D24" s="2">
-        <v>5</v>
-      </c>
-      <c r="E24" s="2">
-        <v>5</v>
-      </c>
-      <c r="F24" s="2">
+      <c r="C24" s="5">
+        <v>5</v>
+      </c>
+      <c r="D24" s="5">
+        <v>5</v>
+      </c>
+      <c r="E24" s="5">
+        <v>5</v>
+      </c>
+      <c r="F24" s="5">
         <v>5</v>
       </c>
       <c r="G24" s="2"/>
@@ -1158,20 +1275,29 @@
       <c r="K24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>22</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="2">
-        <v>5</v>
-      </c>
-      <c r="D25" s="2"/>
-      <c r="E25" s="2"/>
-      <c r="F25" s="2"/>
+      <c r="C25" s="5">
+        <v>5</v>
+      </c>
+      <c r="D25" s="5">
+        <v>0</v>
+      </c>
+      <c r="E25" s="5">
+        <v>0</v>
+      </c>
+      <c r="F25" s="5">
+        <v>0</v>
+      </c>
       <c r="G25" s="2"/>
       <c r="H25" s="2"/>
       <c r="I25" s="2"/>
@@ -1182,18 +1308,29 @@
       <c r="K25">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>23</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="2"/>
-      <c r="D26" s="2"/>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+      <c r="C26" s="5">
+        <v>0</v>
+      </c>
+      <c r="D26" s="5">
+        <v>0</v>
+      </c>
+      <c r="E26" s="5">
+        <v>0</v>
+      </c>
+      <c r="F26" s="5">
+        <v>0</v>
+      </c>
       <c r="G26" s="2"/>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
@@ -1204,24 +1341,27 @@
       <c r="K26">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>24</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="2">
-        <v>5</v>
-      </c>
-      <c r="D27" s="2">
-        <v>5</v>
-      </c>
-      <c r="E27" s="2">
-        <v>5</v>
-      </c>
-      <c r="F27" s="2">
+      <c r="C27" s="5">
+        <v>5</v>
+      </c>
+      <c r="D27" s="5">
+        <v>5</v>
+      </c>
+      <c r="E27" s="5">
+        <v>5</v>
+      </c>
+      <c r="F27" s="5">
         <v>5</v>
       </c>
       <c r="G27" s="2"/>
@@ -1234,24 +1374,27 @@
       <c r="K27">
         <v>5</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>25</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="2">
-        <v>5</v>
-      </c>
-      <c r="D28" s="2">
-        <v>5</v>
-      </c>
-      <c r="E28" s="2">
-        <v>5</v>
-      </c>
-      <c r="F28" s="2">
+      <c r="C28" s="5">
+        <v>5</v>
+      </c>
+      <c r="D28" s="5">
+        <v>5</v>
+      </c>
+      <c r="E28" s="5">
+        <v>5</v>
+      </c>
+      <c r="F28" s="5">
         <v>5</v>
       </c>
       <c r="G28" s="2">
@@ -1266,18 +1409,29 @@
       <c r="K28">
         <v>5</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>26</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="2"/>
-      <c r="D29" s="2"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
+      <c r="C29" s="5">
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <v>0</v>
+      </c>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
@@ -1288,18 +1442,29 @@
       <c r="K29">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>27</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
+      <c r="C30" s="5">
+        <v>0</v>
+      </c>
+      <c r="D30" s="5">
+        <v>0</v>
+      </c>
+      <c r="E30" s="5">
+        <v>0</v>
+      </c>
+      <c r="F30" s="5">
+        <v>0</v>
+      </c>
       <c r="G30" s="2"/>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
@@ -1310,24 +1475,27 @@
       <c r="K30">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>28</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="2">
-        <v>4</v>
-      </c>
-      <c r="D31" s="2">
-        <v>4</v>
-      </c>
-      <c r="E31" s="2">
-        <v>4</v>
-      </c>
-      <c r="F31" s="2">
+      <c r="C31" s="5">
+        <v>4</v>
+      </c>
+      <c r="D31" s="5">
+        <v>4</v>
+      </c>
+      <c r="E31" s="5">
+        <v>4</v>
+      </c>
+      <c r="F31" s="5">
         <v>4</v>
       </c>
       <c r="G31" s="2"/>
@@ -1340,24 +1508,29 @@
       <c r="K31">
         <v>4</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" ht="13" x14ac:dyDescent="0.25">
+      <c r="L31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="13" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>29</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="2">
-        <v>5</v>
-      </c>
-      <c r="D32" s="2">
-        <v>5</v>
-      </c>
-      <c r="E32" s="2">
-        <v>5</v>
-      </c>
-      <c r="F32" s="2"/>
+      <c r="C32" s="5">
+        <v>5</v>
+      </c>
+      <c r="D32" s="5">
+        <v>5</v>
+      </c>
+      <c r="E32" s="5">
+        <v>5</v>
+      </c>
+      <c r="F32" s="5">
+        <v>0</v>
+      </c>
       <c r="G32" s="2"/>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
@@ -1367,6 +1540,9 @@
       </c>
       <c r="K32">
         <v>4</v>
+      </c>
+      <c r="L32">
+        <v>0</v>
       </c>
     </row>
     <row r="33" spans="3:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 22:13:31_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -530,10 +530,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L33" sqref="L33"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1293,7 +1293,7 @@
         <v>0</v>
       </c>
       <c r="E25" s="5">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F25" s="5">
         <v>0</v>
@@ -1303,7 +1303,7 @@
       <c r="I25" s="2"/>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K25">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_11 апреля 2024 г. 22:32:16_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -154,7 +154,7 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -164,6 +164,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -206,7 +212,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -221,6 +227,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -533,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1319,14 +1328,14 @@
       <c r="B26" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="5">
-        <v>0</v>
+      <c r="C26" s="6">
+        <v>5</v>
       </c>
       <c r="D26" s="5">
         <v>0</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
+      <c r="E26" s="6">
+        <v>5</v>
       </c>
       <c r="F26" s="5">
         <v>0</v>
@@ -1336,7 +1345,7 @@
       <c r="I26" s="2"/>
       <c r="J26">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K26">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 8:42:01_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E26" sqref="E26"/>
+      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -739,15 +739,17 @@
       <c r="E8" s="5">
         <v>5</v>
       </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2"/>
+      <c r="F8" s="2">
+        <v>5</v>
+      </c>
+      <c r="G8" s="2">
+        <v>5</v>
+      </c>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
       <c r="J8">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K8">
         <v>4</v>
@@ -901,18 +903,20 @@
       <c r="D13" s="5">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
-        <v>0</v>
-      </c>
-      <c r="F13" s="5">
-        <v>0</v>
-      </c>
-      <c r="G13" s="2"/>
+      <c r="E13" s="2">
+        <v>5</v>
+      </c>
+      <c r="F13" s="2">
+        <v>5</v>
+      </c>
+      <c r="G13" s="2">
+        <v>5</v>
+      </c>
       <c r="H13" s="2"/>
       <c r="I13" s="2"/>
       <c r="J13">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="K13">
         <v>4</v>
@@ -975,12 +979,14 @@
       <c r="F15" s="5">
         <v>5</v>
       </c>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2">
+        <v>5</v>
+      </c>
       <c r="H15" s="2"/>
       <c r="I15" s="2"/>
       <c r="J15">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K15">
         <v>5</v>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 9:47:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A23" sqref="A23"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1113,12 +1113,14 @@
       <c r="F19" s="5">
         <v>5</v>
       </c>
-      <c r="G19" s="2"/>
+      <c r="G19" s="2">
+        <v>5</v>
+      </c>
       <c r="H19" s="2"/>
       <c r="I19" s="2"/>
       <c r="J19">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K19">
         <v>5</v>
@@ -1513,12 +1515,14 @@
       <c r="F31" s="5">
         <v>4</v>
       </c>
-      <c r="G31" s="2"/>
+      <c r="G31" s="2">
+        <v>5</v>
+      </c>
       <c r="H31" s="2"/>
       <c r="I31" s="2"/>
       <c r="J31">
         <f t="shared" si="0"/>
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="K31">
         <v>4</v>
@@ -1543,15 +1547,17 @@
       <c r="E32" s="5">
         <v>5</v>
       </c>
-      <c r="F32" s="5">
-        <v>0</v>
-      </c>
-      <c r="G32" s="2"/>
+      <c r="F32" s="2">
+        <v>5</v>
+      </c>
+      <c r="G32" s="2">
+        <v>5</v>
+      </c>
       <c r="H32" s="2"/>
       <c r="I32" s="2"/>
       <c r="J32">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K32">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 9:48:21_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1211,15 +1211,15 @@
       <c r="E22" s="5">
         <v>5</v>
       </c>
-      <c r="F22" s="5">
-        <v>0</v>
+      <c r="F22" s="2">
+        <v>5</v>
       </c>
       <c r="G22" s="2"/>
       <c r="H22" s="2"/>
       <c r="I22" s="2"/>
       <c r="J22">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K22">
         <v>4</v>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 10:03:28_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="J22" sqref="J22"/>
+      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -582,7 +582,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="1"/>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
@@ -591,15 +591,15 @@
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
     </row>
-    <row r="4" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="5">
-        <v>0</v>
+      <c r="C4" s="2">
+        <v>4</v>
       </c>
       <c r="D4" s="5">
         <v>5</v>
@@ -607,15 +607,14 @@
       <c r="E4" s="5">
         <v>5</v>
       </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2"/>
+      <c r="F4" s="2">
+        <v>4</v>
+      </c>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
       <c r="J4">
         <f>SUM(C4:I4)</f>
-        <v>10</v>
+        <v>18</v>
       </c>
       <c r="K4">
         <v>4</v>
@@ -624,7 +623,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" ht="13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
AutoCommit_12 апреля 2024 г. 10:04:43_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C4" sqref="C4"/>
+      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1436,14 +1436,14 @@
       <c r="B29" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="5">
-        <v>0</v>
-      </c>
-      <c r="D29" s="5">
-        <v>0</v>
-      </c>
-      <c r="E29" s="5">
-        <v>0</v>
+      <c r="C29" s="2">
+        <v>5</v>
+      </c>
+      <c r="D29" s="2">
+        <v>5</v>
+      </c>
+      <c r="E29" s="2">
+        <v>5</v>
       </c>
       <c r="F29" s="5">
         <v>0</v>
@@ -1453,7 +1453,7 @@
       <c r="I29" s="2"/>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="K29">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_19 апреля 2024 г. 8:37:37_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F29" sqref="F29"/>
+      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1013,12 +1013,14 @@
       <c r="F16" s="5">
         <v>5</v>
       </c>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2">
+        <v>5</v>
+      </c>
       <c r="H16" s="2"/>
       <c r="I16" s="2"/>
       <c r="J16">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K16">
         <v>5</v>
@@ -1144,15 +1146,15 @@
       <c r="E20" s="5">
         <v>5</v>
       </c>
-      <c r="F20" s="5">
-        <v>0</v>
+      <c r="F20" s="2">
+        <v>5</v>
       </c>
       <c r="G20" s="2"/>
       <c r="H20" s="2"/>
       <c r="I20" s="2"/>
       <c r="J20">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K20">
         <v>4</v>
@@ -1171,8 +1173,8 @@
       <c r="C21" s="5">
         <v>5</v>
       </c>
-      <c r="D21" s="5">
-        <v>0</v>
+      <c r="D21" s="2">
+        <v>5</v>
       </c>
       <c r="E21" s="5">
         <v>0</v>
@@ -1185,7 +1187,7 @@
       <c r="I21" s="2"/>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_19 апреля 2024 г. 10:01:41_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="G15" sqref="G15"/>
+      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1307,8 +1307,8 @@
       <c r="C25" s="5">
         <v>5</v>
       </c>
-      <c r="D25" s="5">
-        <v>0</v>
+      <c r="D25" s="2">
+        <v>5</v>
       </c>
       <c r="E25" s="5">
         <v>5</v>
@@ -1321,7 +1321,7 @@
       <c r="I25" s="2"/>
       <c r="J25">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K25">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_26 апреля 2024 г. 10:01:10_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -539,10 +539,10 @@
   <dimension ref="A1:L33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <pane xSplit="2" ySplit="3" topLeftCell="C13" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="D25" sqref="D25"/>
+      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -809,12 +809,14 @@
       <c r="F10" s="5">
         <v>5</v>
       </c>
-      <c r="G10" s="2"/>
+      <c r="G10" s="2">
+        <v>5</v>
+      </c>
       <c r="H10" s="2"/>
       <c r="I10" s="2"/>
       <c r="J10">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="K10">
         <v>5</v>
@@ -1176,8 +1178,8 @@
       <c r="D21" s="2">
         <v>5</v>
       </c>
-      <c r="E21" s="5">
-        <v>0</v>
+      <c r="E21" s="2">
+        <v>5</v>
       </c>
       <c r="F21" s="5">
         <v>0</v>
@@ -1187,7 +1189,7 @@
       <c r="I21" s="2"/>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="K21">
         <v>3</v>
@@ -1447,15 +1449,17 @@
       <c r="E29" s="2">
         <v>5</v>
       </c>
-      <c r="F29" s="5">
-        <v>0</v>
-      </c>
-      <c r="G29" s="2"/>
+      <c r="F29" s="2">
+        <v>5</v>
+      </c>
+      <c r="G29" s="2">
+        <v>5</v>
+      </c>
       <c r="H29" s="2"/>
       <c r="I29" s="2"/>
       <c r="J29">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="K29">
         <v>3</v>
@@ -1471,24 +1475,26 @@
       <c r="B30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="5">
-        <v>0</v>
-      </c>
-      <c r="D30" s="5">
-        <v>0</v>
-      </c>
-      <c r="E30" s="5">
-        <v>0</v>
-      </c>
-      <c r="F30" s="5">
-        <v>0</v>
-      </c>
-      <c r="G30" s="2"/>
+      <c r="C30" s="2">
+        <v>5</v>
+      </c>
+      <c r="D30" s="2">
+        <v>5</v>
+      </c>
+      <c r="E30" s="2">
+        <v>5</v>
+      </c>
+      <c r="F30" s="2">
+        <v>5</v>
+      </c>
+      <c r="G30" s="2">
+        <v>5</v>
+      </c>
       <c r="H30" s="2"/>
       <c r="I30" s="2"/>
       <c r="J30">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="K30">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_3 мая 2024 г. 8:35:44_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E21" sqref="E21"/>
+      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1181,15 +1181,15 @@
       <c r="E21" s="2">
         <v>5</v>
       </c>
-      <c r="F21" s="5">
-        <v>0</v>
+      <c r="F21" s="2">
+        <v>5</v>
       </c>
       <c r="G21" s="2"/>
       <c r="H21" s="2"/>
       <c r="I21" s="2"/>
       <c r="J21">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K21">
         <v>3</v>

</xml_diff>

<commit_message>
AutoCommit_3 мая 2024 г. 13:39:33_SibNout2023
</commit_message>
<xml_diff>
--- a/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
+++ b/2ИСИП-522/_2ИСИП-522_ТерВер.xlsx
@@ -542,7 +542,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="F21" sqref="F21"/>
+      <selection pane="bottomRight" activeCell="G9" activeCellId="1" sqref="F9 G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -773,15 +773,15 @@
       <c r="E9" s="5">
         <v>5</v>
       </c>
-      <c r="F9" s="5">
-        <v>0</v>
+      <c r="F9" s="2">
+        <v>5</v>
       </c>
       <c r="G9" s="2"/>
       <c r="H9" s="2"/>
       <c r="I9" s="2"/>
       <c r="J9">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="K9">
         <v>4</v>

</xml_diff>